<commit_message>
Power and turbine data update
Power curve data updated according to the Siemens SWT-6.0-120 version. Turbine rotor diameter shortened to 125m.
</commit_message>
<xml_diff>
--- a/wind_turbine_6MW.xlsx
+++ b/wind_turbine_6MW.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jc17718\Desktop\ATMD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E277DE2-0082-4370-8D72-8D7013DDAF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F423A1D-2753-474A-AF4A-FB57348DC972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="990" yWindow="340" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,16 +48,16 @@
     <t>maximum blade tip height above LAT (m)</t>
   </si>
   <si>
-    <t>maximum rotor blade diameter (m)</t>
+    <t>turbine rating (MW)</t>
   </si>
   <si>
-    <t>turbine rating (MW)</t>
+    <t>rotor blade diameter (m)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -477,11 +477,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -504,7 +504,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>6</v>
@@ -528,10 +528,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>265</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>